<commit_message>
chore: convertion from string to int
</commit_message>
<xml_diff>
--- a/data/test_db.xlsx
+++ b/data/test_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\DBMS-master-python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D17B51-0C85-4834-AE9A-66B586B69FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9CB48C-6B20-427D-8D2E-DAEB6CD3F161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="2670" windowWidth="16875" windowHeight="10432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="2670" windowWidth="16875" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -21,33 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>v3</t>
   </si>
   <si>
     <t>v2</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
   <si>
     <t>v1</t>
@@ -120,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -426,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -441,59 +421,59 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -515,18 +495,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -537,7 +517,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -548,7 +528,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -559,7 +539,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -570,7 +550,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>4</v>

</xml_diff>